<commit_message>
plots for submission and confusion matrix
</commit_message>
<xml_diff>
--- a/plots/confusion/confusion.xlsx
+++ b/plots/confusion/confusion.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="37820" yWindow="6640" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="confusion" localSheetId="0">Sheet3!$A$1:$H$23</definedName>
+    <definedName name="confusion" localSheetId="1">Sheet3!$A$1:$H$23</definedName>
+    <definedName name="confusion_matrix_b" localSheetId="0">Sheet2!$A$1:$K$15</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,8 +25,22 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="confusion.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:dealmaker:Desktop:confusion.csv" delimited="0" comma="1">
+  <connection id="1" name="confusion_matrix_b.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:dealmaker:projects:cs229_project:229-Final:plots:confusion:confusion_matrix_b.csv" space="1" comma="1" consecutive="1">
+      <textFields count="8">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="confusion.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:dealmaker:Desktop:confusion.csv" delimited="0" comma="1">
       <textFields count="12">
         <textField/>
         <textField position="14"/>
@@ -41,8 +57,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="confusion.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:dealmaker:Desktop:confusion.csv" delimited="0" comma="1">
+  <connection id="3" name="confusion.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:dealmaker:Desktop:confusion.csv" delimited="0" comma="1">
       <textFields count="8">
         <textField/>
         <textField position="15"/>
@@ -55,8 +71,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="confusion.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:dealmaker:Desktop:confusion.csv" delimited="0" comma="1">
+  <connection id="4" name="confusion.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:dealmaker:Desktop:confusion.csv" delimited="0" comma="1">
       <textFields count="8">
         <textField/>
         <textField position="15"/>
@@ -73,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>void</t>
   </si>
@@ -109,6 +125,42 @@
   </si>
   <si>
     <t>For dataset train</t>
+  </si>
+  <si>
+    <t>GPUB</t>
+  </si>
+  <si>
+    <t>python3</t>
+  </si>
+  <si>
+    <t>main.py</t>
+  </si>
+  <si>
+    <t>Â --num-batches-train</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Finished.</t>
+  </si>
+  <si>
+    <t>Saving</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>to:</t>
+  </si>
+  <si>
+    <t>./runs/1513034153.3755772/test</t>
+  </si>
+  <si>
+    <t>./runs/1513036475.4784913/train</t>
   </si>
 </sst>
 </file>
@@ -172,7 +224,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -195,13 +247,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -212,6 +277,12 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -222,6 +293,12 @@
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -231,7 +308,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="confusion" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="confusion_matrix_b" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="confusion" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -556,10 +637,442 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="8" width="6.83203125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="6.83203125" customWidth="1"/>
+    <col min="11" max="14" width="9.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="21" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="21" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="e">
+        <f>--epochs</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D2" s="1">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="e">
+        <f>--scale-factor</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="e">
+        <f>--no-early-stop</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>744</v>
+      </c>
+      <c r="J2" t="e">
+        <f>--save-test</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K2" t="e">
+        <f>--save-train</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="21" customHeight="1"/>
+    <row r="4" spans="1:11" ht="21" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="21" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="21" customHeight="1">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>4</v>
+      </c>
+      <c r="I6" s="3">
+        <v>5</v>
+      </c>
+      <c r="J6" s="3">
+        <v>6</v>
+      </c>
+      <c r="K6" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="21" customHeight="1">
+      <c r="B7"/>
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="1:11" ht="21" customHeight="1">
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="21" customHeight="1">
+      <c r="A9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.69382514100000003</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.13833564300000001</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.106046063</v>
+      </c>
+      <c r="G9" s="1">
+        <v>7.4735919399999996E-3</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3.3009956E-2</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5.92167445E-3</v>
+      </c>
+      <c r="J9" s="1">
+        <v>5.1009064700000004E-3</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.0287023899999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="21" customHeight="1">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4.8084720300000001E-3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.96977671799999998</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6.7740925400000002E-3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.1835232200000001E-3</v>
+      </c>
+      <c r="H10" s="1">
+        <v>8.6496294699999997E-3</v>
+      </c>
+      <c r="I10" s="1">
+        <v>7.2901863500000004E-5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.8026350700000001E-3</v>
+      </c>
+      <c r="K10" s="1">
+        <v>5.9320278400000004E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="21" customHeight="1">
+      <c r="A11" s="3">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2.0833352E-3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9.2433616999999992E-3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.91087473500000005</v>
+      </c>
+      <c r="G11" s="1">
+        <v>5.4900111399999998E-3</v>
+      </c>
+      <c r="H11" s="1">
+        <v>4.9083747900000002E-2</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1.53275014E-2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2.4458492700000002E-3</v>
+      </c>
+      <c r="K11" s="1">
+        <v>5.4514585299999998E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="21" customHeight="1">
+      <c r="A12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>7.1009450999999996E-3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3.8383325599999997E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.44696537600000003</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.239706168</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.21423772299999999</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1.45363334E-2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1.42884871E-2</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2.47816415E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="21" customHeight="1">
+      <c r="A13" s="3">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6.3153337899999999E-4</v>
+      </c>
+      <c r="E13" s="1">
+        <v>5.5637664800000002E-3</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5.9294440499999997E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4.2058341900000004E-3</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.92235663000000001</v>
+      </c>
+      <c r="I13" s="1">
+        <v>4.5264409600000001E-3</v>
+      </c>
+      <c r="J13" s="1">
+        <v>7.4343598299999995E-4</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2.6779183599999999E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="21" customHeight="1">
+      <c r="A14" s="3">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4.0585702399999999E-4</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4.2276773399999997E-6</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2.72051037E-2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2.6232737900000001E-3</v>
+      </c>
+      <c r="H14" s="1">
+        <v>3.6279813100000002E-2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.933439448</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>4.2276773400000001E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="21" customHeight="1">
+      <c r="A15" s="3">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.7096436199999996E-3</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5.3791581900000003E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.302061841</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2.6591153499999999E-2</v>
+      </c>
+      <c r="H15" s="1">
+        <v>5.4871660000000003E-2</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1.38471551E-4</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.49048931200000001</v>
+      </c>
+      <c r="K15" s="1">
+        <v>6.6346335800000003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="21" customHeight="1">
+      <c r="A16" s="3">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2.90052025E-3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2.5487202099999998E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>9.1461981100000006E-2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>3.5171391600000001E-3</v>
+      </c>
+      <c r="H16" s="1">
+        <v>3.33008661E-2</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3.14768454E-3</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1.54128892E-2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.82477171800000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="A17:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>